<commit_message>
Add comments to archive jobs on AZU-SQL-01 and -02
</commit_message>
<xml_diff>
--- a/ACTIVE/Updated AZU-SQL-01/Updated AZU-SQL-01.xlsx
+++ b/ACTIVE/Updated AZU-SQL-01/Updated AZU-SQL-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkaja\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rglazebrook\source\repos\Application Support\ACTIVE\Updated AZU-SQL-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC0F26F-DE52-4B23-BFAC-55CE2DB91748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F193EB13-8538-42FB-BB95-F413A9A62E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA0B3705-C37B-4371-A7EA-937BAA35C107}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA0B3705-C37B-4371-A7EA-937BAA35C107}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="102">
   <si>
     <t>JOB ID</t>
   </si>
@@ -339,6 +337,12 @@
   </si>
   <si>
     <t>Occurs every day at 2:00:00 AM. Schedule will be used starting on 1/1/2008.</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Archive</t>
   </si>
 </sst>
 </file>
@@ -368,12 +372,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -388,10 +398,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,32 +717,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AA6ECA-E920-40B8-9A15-F69B0D1EADA0}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" customWidth="1"/>
-    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.26953125" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.21875" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.81640625" customWidth="1"/>
-    <col min="14" max="14" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" customWidth="1"/>
-    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.77734375" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.21875" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -783,8 +794,11 @@
       <c r="Q1" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R1" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -825,7 +839,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -866,7 +880,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -907,7 +921,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -948,7 +962,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -989,7 +1003,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1036,7 +1050,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1083,7 +1097,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1130,7 +1144,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1177,7 +1191,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -1218,7 +1232,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -1258,8 +1272,11 @@
       <c r="Q12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1299,8 +1316,11 @@
       <c r="Q13" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1340,8 +1360,11 @@
       <c r="Q14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1388,7 +1411,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1429,7 +1452,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1470,7 +1493,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1564,7 +1587,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Updated comments to archive jobs
</commit_message>
<xml_diff>
--- a/ACTIVE/Updated AZU-SQL-01/Updated AZU-SQL-01.xlsx
+++ b/ACTIVE/Updated AZU-SQL-01/Updated AZU-SQL-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rglazebrook\source\repos\Application Support\ACTIVE\Updated AZU-SQL-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F193EB13-8538-42FB-BB95-F413A9A62E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13981AFB-CA45-4127-8047-E5FC6EF8D86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA0B3705-C37B-4371-A7EA-937BAA35C107}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="103">
   <si>
     <t>JOB ID</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Archive</t>
+  </si>
+  <si>
+    <t>Dee to review</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,6 +841,9 @@
       <c r="Q2" t="s">
         <v>83</v>
       </c>
+      <c r="R2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -879,6 +885,9 @@
       <c r="Q3" t="s">
         <v>83</v>
       </c>
+      <c r="R3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -920,6 +929,9 @@
       <c r="Q4" t="s">
         <v>83</v>
       </c>
+      <c r="R4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -961,6 +973,9 @@
       <c r="Q5" t="s">
         <v>83</v>
       </c>
+      <c r="R5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1002,6 +1017,9 @@
       <c r="Q6" t="s">
         <v>83</v>
       </c>
+      <c r="R6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1230,6 +1248,9 @@
       </c>
       <c r="Q11" t="s">
         <v>83</v>
+      </c>
+      <c r="R11" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>